<commit_message>
fixed remaining duplicate term
</commit_message>
<xml_diff>
--- a/mvreason.xlsx
+++ b/mvreason.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693361EA-AAC6-E643-89CA-19A187933441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68E58B7-5D83-5743-854F-2CDF9A016D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12240" yWindow="5980" windowWidth="35200" windowHeight="21720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Record Not Provided</t>
   </si>
   <si>
-    <t>Element Never Collected</t>
-  </si>
-  <si>
     <t>CDE Omitted with Exception</t>
   </si>
   <si>
@@ -346,6 +343,12 @@
   </si>
   <si>
     <t>This information was not provided by the participant or sensor</t>
+  </si>
+  <si>
+    <t>Element Never Presented for Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Originators Omitted Element </t>
   </si>
 </sst>
 </file>
@@ -775,8 +778,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -863,7 +866,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -871,7 +874,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,7 +890,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -895,7 +898,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
@@ -962,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -984,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" s="5" t="str">
         <f>A$21</f>
@@ -1009,7 +1012,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" s="7" t="str">
         <f>A$22</f>
@@ -1026,7 +1029,7 @@
         <v>mvreason:NoParticipantConsenttoShare</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>45</v>
@@ -1141,13 +1144,13 @@
         <v>mvreason:OtherUnsentReasonNotSpecified</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1170,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="5" t="str">
         <f>A$21</f>
@@ -1197,7 +1200,7 @@
         <v>51</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="7" t="str">
         <f>A$30</f>
@@ -1220,7 +1223,7 @@
         <v>52</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32" s="7" t="str">
         <f>A$31</f>
@@ -1243,7 +1246,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" s="7" t="str">
         <f>A$31</f>
@@ -1266,7 +1269,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34" s="7" t="str">
         <f>A$31</f>
@@ -1289,7 +1292,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E35" s="7" t="str">
         <f t="shared" ref="E35:E38" si="3">A$30</f>
@@ -1303,16 +1306,16 @@
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:ElementNeverCollected</v>
+        <v>mvreason:AllOriginatorsOmittedElement</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>56</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E36" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1329,13 +1332,13 @@
         <v>mvreason:CDEOmittedwithException</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>57</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E37" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1352,13 +1355,13 @@
         <v>mvreason:OtherUnenteredReasonNotSpecified</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>58</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E38" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1381,7 +1384,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" s="5" t="str">
         <f>A$21</f>
@@ -1402,13 +1405,13 @@
         <v>mvreason:SkipLogic</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>59</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E40" s="7" t="str">
         <f>A$39</f>
@@ -1425,7 +1428,7 @@
         <v>mvreason:NoParticipantConsenttoAsk</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="25" t="s">
         <v>60</v>
@@ -1445,16 +1448,16 @@
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>mvreason:ElementNeverCollected</v>
+        <v>mvreason:ElementNeverPresentedforCollection</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C42" s="25" t="s">
         <v>61</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" s="7" t="str">
         <f t="shared" ref="E42:E43" si="6">A$39</f>
@@ -1471,13 +1474,13 @@
         <v>mvreason:ProcessError</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" s="7" t="str">
         <f t="shared" si="6"/>
@@ -1494,13 +1497,13 @@
         <v>mvreason:OtherUnpresentedReasonNotSpecified</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E44" s="7" t="str">
         <f t="shared" ref="E44" si="9">A$39</f>

</xml_diff>

<commit_message>
additional normalization to 0.0.4
</commit_message>
<xml_diff>
--- a/mvreason.xlsx
+++ b/mvreason.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F7CE4C-C00E-044B-91BB-9176BE0C5398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E105D83-85DA-E94B-9E00-926EC66AF4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12240" yWindow="5980" windowWidth="35200" windowHeight="21720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Extend the equation in column A down to include all the rows that are filled out. Verify that any special characters in the prefLabel are replaced by hyphens or other IRI-compatible ASCII characters.</t>
   </si>
   <si>
-    <t>In this spreadsheet, the identifier column gets filled out automatcially from the skos:prefLabel column. You can choose to replace any of the auto-generated identifiers.</t>
-  </si>
-  <si>
     <t>https://radx.orgx/vocs/missing-value-reason</t>
   </si>
   <si>
@@ -150,21 +147,6 @@
     <t>Not Presented to Participant</t>
   </si>
   <si>
-    <t>participant did not consent to its being provided</t>
-  </si>
-  <si>
-    <t>not available or mappable from data source</t>
-  </si>
-  <si>
-    <t>data lost or inaccessible (unspecified reason)</t>
-  </si>
-  <si>
-    <t>data invalid (wrong format, wrong or unknown units, not parseable, impossible value)</t>
-  </si>
-  <si>
-    <t>data anonymization/privacy concerns</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -252,18 +234,12 @@
     <t>CDE Omitted with Exception</t>
   </si>
   <si>
-    <t>Skip Logic</t>
-  </si>
-  <si>
     <t>Process Error</t>
   </si>
   <si>
     <t>This question (element) was not presented to the participant</t>
   </si>
   <si>
-    <t>This information was not sent by the aggregator to the Data Hub</t>
-  </si>
-  <si>
     <t>Reason for the data not being available is not known</t>
   </si>
   <si>
@@ -282,9 +258,6 @@
     <t xml:space="preserve">https://orcid.org/0000-0002-9381-9693 </t>
   </si>
   <si>
-    <t>data originator's data transfer agreement with project precluded sending</t>
-  </si>
-  <si>
     <t>Other Unsent Reason Not Specified</t>
   </si>
   <si>
@@ -294,61 +267,100 @@
     <t>Other Unpresented Reason Not Specified</t>
   </si>
   <si>
-    <t>other unsent reason not specified</t>
-  </si>
-  <si>
-    <t>other unpresented reason not specified</t>
-  </si>
-  <si>
     <t>3e</t>
   </si>
   <si>
-    <t>originator omitted this value</t>
-  </si>
-  <si>
-    <t>originator chose not to answer for personal reasons (unknown to data collector)</t>
-  </si>
-  <si>
-    <t>originator deemed the question not applicable</t>
-  </si>
-  <si>
-    <t>originator did not know the answer</t>
-  </si>
-  <si>
-    <t>originator omitted this row (did not provide any answers for this record)</t>
-  </si>
-  <si>
-    <t>originator omitted this column/variable (this column/variable was not collected or could not be collected for any user</t>
-  </si>
-  <si>
-    <t>originator omitted this CDE (category) due to NIH-approved exception</t>
-  </si>
-  <si>
-    <t>originator did not provide data for other unentered reason not specified</t>
-  </si>
-  <si>
-    <t>column (variable) not presented for collection</t>
-  </si>
-  <si>
-    <t>processing error caused question to not be presented</t>
-  </si>
-  <si>
-    <t>skip logic caused question to not be presented</t>
-  </si>
-  <si>
-    <t>2022-03-14T22:16:17-08:01</t>
-  </si>
-  <si>
-    <t>This information was not provided by the participant or sensor</t>
-  </si>
-  <si>
     <t>Element Never Presented for Collection</t>
   </si>
   <si>
     <t xml:space="preserve">All Originators Omitted Element </t>
   </si>
   <si>
-    <t>0.0.3</t>
+    <t>Originator did not consent to its being provided</t>
+  </si>
+  <si>
+    <t>Data originator's data transfer agreement with project precluded sending</t>
+  </si>
+  <si>
+    <t>Reason from the originator was not available or mappable</t>
+  </si>
+  <si>
+    <t>Data was lost or inaccessible (unspecified reason)</t>
+  </si>
+  <si>
+    <t>Data was invalid (wrong format, wrong or unknown units, not parseable, or impossible value)</t>
+  </si>
+  <si>
+    <t>Data had anonymization/privacy concerns</t>
+  </si>
+  <si>
+    <t>Originator chose not to answer for personal reasons (unknown to data collector)</t>
+  </si>
+  <si>
+    <t>Originator deemed the question not applicable</t>
+  </si>
+  <si>
+    <t>Originator did not know the answer</t>
+  </si>
+  <si>
+    <t>Originator omitted this row (did not provide any answers for this record)</t>
+  </si>
+  <si>
+    <t>Originator omitted this column/variable (this column/variable was not collected or could not be collected for any user</t>
+  </si>
+  <si>
+    <t>Originator omitted this CDE (category) due to NIH-approved exception</t>
+  </si>
+  <si>
+    <t>Originator did not provide data for some other reason</t>
+  </si>
+  <si>
+    <t>Originator did not provide consent for question to be asked</t>
+  </si>
+  <si>
+    <t>The CDE (or element of the CDE) was not presented due to CDE exception</t>
+  </si>
+  <si>
+    <t>This element (question or variable) was not presented to user for collection (reason unspecified)</t>
+  </si>
+  <si>
+    <t>3f</t>
+  </si>
+  <si>
+    <t>CDE Not Presented Due to Exception</t>
+  </si>
+  <si>
+    <t>0.0.4</t>
+  </si>
+  <si>
+    <t>In this spreadsheet, the identifier column gets filled out automatically from the skos:prefLabel column. You can choose to replace any of the auto-generated identifiers.</t>
+  </si>
+  <si>
+    <t>Originator omitted this particular value. (If column, record, or CDE omitted *by the user*, choose that appropriate term here.)</t>
+  </si>
+  <si>
+    <t>Skipped by Form Logic</t>
+  </si>
+  <si>
+    <t>Skip logic in the form or directions caused the question to not be presented</t>
+  </si>
+  <si>
+    <t>A processing error caused the question to not be presented</t>
+  </si>
+  <si>
+    <t>Data was not sent to Data Hub for some  reason not specified</t>
+  </si>
+  <si>
+    <t>Question was not presented for some reason not specified</t>
+  </si>
+  <si>
+    <t>2022-03-20T21:39:00-08:00</t>
+  </si>
+  <si>
+    <t>This information was not provided by the originator (participant or sensor)</t>
+  </si>
+  <si>
+    <t>This information was not sent by the data aggregator (e.g., the Data Coordination Center) to the Data Hub</t>
   </si>
 </sst>
 </file>
@@ -776,10 +788,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -801,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -809,10 +821,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -842,7 +854,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -850,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -858,7 +870,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -866,7 +878,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -874,7 +886,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -890,7 +902,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -898,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
@@ -921,7 +933,7 @@
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -959,13 +971,13 @@
         <v>mvreason:ReasonUnknown</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="23">
         <v>0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -981,13 +993,13 @@
         <v>mvreason:NotSenttoDataHub</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="23">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E22" s="5" t="str">
         <f>A$21</f>
@@ -1006,13 +1018,13 @@
         <v>mvreason:DataTransferAgreement</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="7" t="str">
         <f>A$22</f>
@@ -1029,13 +1041,13 @@
         <v>mvreason:NoParticipantConsenttoShare</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="E24" s="7" t="str">
         <f t="shared" ref="E24:E29" si="1">A$22</f>
@@ -1052,13 +1064,13 @@
         <v>mvreason:NotAvailableOrMappable</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E25" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1075,13 +1087,13 @@
         <v>mvreason:DataLostOrInaccessible</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="E26" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1098,13 +1110,13 @@
         <v>mvreason:DataInvalid</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="E27" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1121,13 +1133,13 @@
         <v>mvreason:AnonymizationOrPrivacyConcerns</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E28" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1144,13 +1156,13 @@
         <v>mvreason:OtherUnsentReasonNotSpecified</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E29" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1167,13 +1179,13 @@
         <v>mvreason:NotEnteredByOriginator</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="23">
         <v>2</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E30" s="5" t="str">
         <f>A$21</f>
@@ -1194,13 +1206,13 @@
         <v>mvreason:OmittedThisValue</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E31" s="7" t="str">
         <f>A$30</f>
@@ -1217,13 +1229,13 @@
         <v>mvreason:OriginatorChosetoOmit</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E32" s="7" t="str">
         <f>A$31</f>
@@ -1240,13 +1252,13 @@
         <v>mvreason:QuestionNotApplicable</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E33" s="7" t="str">
         <f>A$31</f>
@@ -1263,13 +1275,13 @@
         <v>mvreason:AnswerNotKnown</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E34" s="7" t="str">
         <f>A$31</f>
@@ -1286,13 +1298,13 @@
         <v>mvreason:RecordNotProvided</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E35" s="7" t="str">
         <f t="shared" ref="E35:E38" si="3">A$30</f>
@@ -1309,13 +1321,13 @@
         <v>mvreason:AllOriginatorsOmittedElement</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E36" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1332,13 +1344,13 @@
         <v>mvreason:CDEOmittedwithException</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E37" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1355,13 +1367,13 @@
         <v>mvreason:OtherUnenteredReasonNotSpecified</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E38" s="7" t="str">
         <f t="shared" si="3"/>
@@ -1378,13 +1390,13 @@
         <v>mvreason:NotPresentedtoParticipant</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="26">
         <v>3</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E39" s="5" t="str">
         <f>A$21</f>
@@ -1401,17 +1413,17 @@
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="str">
-        <f t="shared" ref="A40:A42" si="4">IF(ISBLANK($B40),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B40," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:SkipLogic</v>
+        <f t="shared" ref="A40:A43" si="4">IF(ISBLANK($B40),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B40," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>mvreason:SkippedbyFormLogic</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E40" s="7" t="str">
         <f>A$39</f>
@@ -1424,17 +1436,17 @@
     </row>
     <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="str">
-        <f t="shared" ref="A41" si="5">IF(ISBLANK($B41),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B41," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A41:A42" si="5">IF(ISBLANK($B41),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B41," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>mvreason:NoParticipantConsenttoAsk</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E41" s="7" t="str">
         <f>A$39</f>
@@ -1447,20 +1459,20 @@
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>mvreason:ElementNeverPresentedforCollection</v>
+        <f t="shared" si="5"/>
+        <v>mvreason:CDENotPresentedDuetoException</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E42" s="7" t="str">
-        <f t="shared" ref="E42:E43" si="6">A$39</f>
+        <f>A$39</f>
         <v>mvreason:NotPresentedtoParticipant</v>
       </c>
       <c r="F42" s="9"/>
@@ -1470,49 +1482,72 @@
     </row>
     <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="str">
-        <f t="shared" ref="A43" si="7">IF(ISBLANK($B43),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B43," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:ProcessError</v>
+        <f t="shared" si="4"/>
+        <v>mvreason:ElementNeverPresentedforCollection</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E43" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E43:E44" si="6">A$39</f>
         <v>mvreason:NotPresentedtoParticipant</v>
       </c>
-      <c r="F43" s="6"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="8"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="str">
-        <f t="shared" ref="A44" si="8">IF(ISBLANK($B44),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B44," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:OtherUnpresentedReasonNotSpecified</v>
+        <f t="shared" ref="A44" si="7">IF(ISBLANK($B44),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B44," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>mvreason:ProcessError</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44" si="9">A$39</f>
+        <f t="shared" si="6"/>
         <v>mvreason:NotPresentedtoParticipant</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="8"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="str">
+        <f t="shared" ref="A45" si="8">IF(ISBLANK($B45),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B45," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>mvreason:OtherUnpresentedReasonNotSpecified</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f t="shared" ref="E45" si="9">A$39</f>
+        <v>mvreason:NotPresentedtoParticipant</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
0.0.5 with -99xx codes
</commit_message>
<xml_diff>
--- a/mvreason.xlsx
+++ b/mvreason.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Documents/GitHub/excel2rdf-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E105D83-85DA-E94B-9E00-926EC66AF4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA594C8-D1CF-AF40-ADF0-1EEF2AB5332D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12240" yWindow="5980" windowWidth="35200" windowHeight="21720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,18 +135,6 @@
     <t>2022-03-11T22:10:00-08:00</t>
   </si>
   <si>
-    <t>Reason Unknown</t>
-  </si>
-  <si>
-    <t>Not Sent to Data Hub</t>
-  </si>
-  <si>
-    <t>Not Entered By Originator</t>
-  </si>
-  <si>
-    <t>Not Presented to Participant</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -201,42 +189,6 @@
     <t>3c</t>
   </si>
   <si>
-    <t>Data Transfer Agreement</t>
-  </si>
-  <si>
-    <t>Not Available Or Mappable</t>
-  </si>
-  <si>
-    <t>Data Lost Or Inaccessible</t>
-  </si>
-  <si>
-    <t>Data Invalid</t>
-  </si>
-  <si>
-    <t>Anonymization Or Privacy Concerns</t>
-  </si>
-  <si>
-    <t>Omitted This Value</t>
-  </si>
-  <si>
-    <t>Answer Not Known</t>
-  </si>
-  <si>
-    <t>Question Not Applicable</t>
-  </si>
-  <si>
-    <t>Originator Chose to Omit</t>
-  </si>
-  <si>
-    <t>Record Not Provided</t>
-  </si>
-  <si>
-    <t>CDE Omitted with Exception</t>
-  </si>
-  <si>
-    <t>Process Error</t>
-  </si>
-  <si>
     <t>This question (element) was not presented to the participant</t>
   </si>
   <si>
@@ -246,36 +198,15 @@
     <t>3d</t>
   </si>
   <si>
-    <t>No Participant Consent to Ask</t>
-  </si>
-  <si>
-    <t>No Participant Consent to Share</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://orcid.org/0000-0001-6875-5360 </t>
   </si>
   <si>
     <t xml:space="preserve">https://orcid.org/0000-0002-9381-9693 </t>
   </si>
   <si>
-    <t>Other Unsent Reason Not Specified</t>
-  </si>
-  <si>
-    <t>Other Unentered Reason Not Specified</t>
-  </si>
-  <si>
-    <t>Other Unpresented Reason Not Specified</t>
-  </si>
-  <si>
     <t>3e</t>
   </si>
   <si>
-    <t>Element Never Presented for Collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All Originators Omitted Element </t>
-  </si>
-  <si>
     <t>Originator did not consent to its being provided</t>
   </si>
   <si>
@@ -327,21 +258,12 @@
     <t>3f</t>
   </si>
   <si>
-    <t>CDE Not Presented Due to Exception</t>
-  </si>
-  <si>
-    <t>0.0.4</t>
-  </si>
-  <si>
     <t>In this spreadsheet, the identifier column gets filled out automatically from the skos:prefLabel column. You can choose to replace any of the auto-generated identifiers.</t>
   </si>
   <si>
     <t>Originator omitted this particular value. (If column, record, or CDE omitted *by the user*, choose that appropriate term here.)</t>
   </si>
   <si>
-    <t>Skipped by Form Logic</t>
-  </si>
-  <si>
     <t>Skip logic in the form or directions caused the question to not be presented</t>
   </si>
   <si>
@@ -354,13 +276,91 @@
     <t>Question was not presented for some reason not specified</t>
   </si>
   <si>
-    <t>2022-03-20T21:39:00-08:00</t>
-  </si>
-  <si>
     <t>This information was not provided by the originator (participant or sensor)</t>
   </si>
   <si>
     <t>This information was not sent by the data aggregator (e.g., the Data Coordination Center) to the Data Hub</t>
+  </si>
+  <si>
+    <t>Reason Unknown (-9999)</t>
+  </si>
+  <si>
+    <t>Not Sent to Data Hub (-9980)</t>
+  </si>
+  <si>
+    <t>Data Transfer Agreement (-9981)</t>
+  </si>
+  <si>
+    <t>No Participant Consent to Share (-9982)</t>
+  </si>
+  <si>
+    <t>Not Available Or Mappable (-9983)</t>
+  </si>
+  <si>
+    <t>Data Lost Or Inaccessible (-9984)</t>
+  </si>
+  <si>
+    <t>Data Invalid (-9985)</t>
+  </si>
+  <si>
+    <t>Anonymization Or Privacy Concerns (-9986)</t>
+  </si>
+  <si>
+    <t>Other Unsent Reason Not Specified (-9987)</t>
+  </si>
+  <si>
+    <t>Not Entered By Originator (-9960)</t>
+  </si>
+  <si>
+    <t>Omitted This Value (-9961)</t>
+  </si>
+  <si>
+    <t>Originator Chose to Omit (-9962)</t>
+  </si>
+  <si>
+    <t>Question Not Applicable (-9963)</t>
+  </si>
+  <si>
+    <t>Answer Not Known (-9964)</t>
+  </si>
+  <si>
+    <t>Record Not Provided (-9965)</t>
+  </si>
+  <si>
+    <t>All Originators Omitted Element (-9966)</t>
+  </si>
+  <si>
+    <t>CDE Omitted with Exception (-9967)</t>
+  </si>
+  <si>
+    <t>Other Unentered Reason Not Specified (-9968)</t>
+  </si>
+  <si>
+    <t>Not Presented to Participant (-9940)</t>
+  </si>
+  <si>
+    <t>Skip Logic (-9941)</t>
+  </si>
+  <si>
+    <t>No Participant Consent to Ask (-9942)</t>
+  </si>
+  <si>
+    <t>CDE Not Presented Due to Exception (-9943)</t>
+  </si>
+  <si>
+    <t>Element Never Presented for Collection (-9944)</t>
+  </si>
+  <si>
+    <t>Process Error (-9945)</t>
+  </si>
+  <si>
+    <t>Other Unpresented Reason Not Specified (-9946)</t>
+  </si>
+  <si>
+    <t>0.0.5</t>
+  </si>
+  <si>
+    <t>2022-03-23T15:01:00-08:00</t>
   </si>
 </sst>
 </file>
@@ -791,7 +791,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -878,7 +878,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -968,16 +968,16 @@
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="str">
         <f>IF(ISBLANK($B21),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:ReasonUnknown</v>
+        <v>mvreason:ReasonUnknown-9999</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C21" s="23">
         <v>0</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -990,20 +990,20 @@
     <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="str">
         <f t="shared" ref="A22:A39" si="0">IF(ISBLANK($B22),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C22" s="23">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E22" s="5" t="str">
         <f>A$21</f>
-        <v>mvreason:ReasonUnknown</v>
+        <v>mvreason:ReasonUnknown-9999</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>22</v>
@@ -1015,20 +1015,20 @@
     <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:DataTransferAgreement</v>
+        <v>mvreason:DataTransferAgreement-9981</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="E23" s="7" t="str">
         <f>A$22</f>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="27"/>
@@ -1038,20 +1038,20 @@
     <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:NoParticipantConsenttoShare</v>
+        <v>mvreason:NoParticipantConsenttoShare-9982</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E24" s="7" t="str">
         <f t="shared" ref="E24:E29" si="1">A$22</f>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8"/>
@@ -1061,20 +1061,20 @@
     <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:NotAvailableOrMappable</v>
+        <v>mvreason:NotAvailableOrMappable-9983</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E25" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -1084,20 +1084,20 @@
     <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:DataLostOrInaccessible</v>
+        <v>mvreason:DataLostOrInaccessible-9984</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E26" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
@@ -1107,20 +1107,20 @@
     <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:DataInvalid</v>
+        <v>mvreason:DataInvalid-9985</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E27" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="8"/>
@@ -1130,20 +1130,20 @@
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:AnonymizationOrPrivacyConcerns</v>
+        <v>mvreason:AnonymizationOrPrivacyConcerns-9986</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="E28" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="8"/>
@@ -1153,20 +1153,20 @@
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:OtherUnsentReasonNotSpecified</v>
+        <v>mvreason:OtherUnsentReasonNotSpecified-9987</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E29" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>mvreason:NotSenttoDataHub</v>
+        <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="8"/>
@@ -1176,20 +1176,20 @@
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="str">
         <f t="shared" ref="A30" si="2">IF(ISBLANK($B30),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B30," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C30" s="23">
         <v>2</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="E30" s="5" t="str">
         <f>A$21</f>
-        <v>mvreason:ReasonUnknown</v>
+        <v>mvreason:ReasonUnknown-9999</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>22</v>
@@ -1203,20 +1203,20 @@
     <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:OmittedThisValue</v>
+        <v>mvreason:OmittedThisValue-9961</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E31" s="7" t="str">
         <f>A$30</f>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="8"/>
@@ -1226,20 +1226,20 @@
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:OriginatorChosetoOmit</v>
+        <v>mvreason:OriginatorChosetoOmit-9962</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="E32" s="7" t="str">
         <f>A$31</f>
-        <v>mvreason:OmittedThisValue</v>
+        <v>mvreason:OmittedThisValue-9961</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="8"/>
@@ -1249,20 +1249,20 @@
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:QuestionNotApplicable</v>
+        <v>mvreason:QuestionNotApplicable-9963</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E33" s="7" t="str">
         <f>A$31</f>
-        <v>mvreason:OmittedThisValue</v>
+        <v>mvreason:OmittedThisValue-9961</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="8"/>
@@ -1272,20 +1272,20 @@
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:AnswerNotKnown</v>
+        <v>mvreason:AnswerNotKnown-9964</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E34" s="7" t="str">
         <f>A$31</f>
-        <v>mvreason:OmittedThisValue</v>
+        <v>mvreason:OmittedThisValue-9961</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="8"/>
@@ -1295,20 +1295,20 @@
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:RecordNotProvided</v>
+        <v>mvreason:RecordNotProvided-9965</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E35" s="7" t="str">
         <f t="shared" ref="E35:E38" si="3">A$30</f>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="8"/>
@@ -1318,20 +1318,20 @@
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:AllOriginatorsOmittedElement</v>
+        <v>mvreason:AllOriginatorsOmittedElement-9966</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E36" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="8"/>
@@ -1341,20 +1341,20 @@
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:CDEOmittedwithException</v>
+        <v>mvreason:CDEOmittedwithException-9967</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="E37" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="8"/>
@@ -1364,20 +1364,20 @@
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:OtherUnenteredReasonNotSpecified</v>
+        <v>mvreason:OtherUnenteredReasonNotSpecified-9968</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E38" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>mvreason:NotEnteredByOriginator</v>
+        <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8"/>
@@ -1387,20 +1387,20 @@
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="C39" s="26">
         <v>3</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E39" s="5" t="str">
         <f>A$21</f>
-        <v>mvreason:ReasonUnknown</v>
+        <v>mvreason:ReasonUnknown-9999</v>
       </c>
       <c r="F39" s="22" t="s">
         <v>22</v>
@@ -1414,20 +1414,20 @@
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="str">
         <f t="shared" ref="A40:A43" si="4">IF(ISBLANK($B40),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B40," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:SkippedbyFormLogic</v>
+        <v>mvreason:SkipLogic-9941</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>102</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E40" s="7" t="str">
         <f>A$39</f>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="8"/>
@@ -1437,20 +1437,20 @@
     <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="str">
         <f t="shared" ref="A41:A42" si="5">IF(ISBLANK($B41),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B41," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:NoParticipantConsenttoAsk</v>
+        <v>mvreason:NoParticipantConsenttoAsk-9942</v>
       </c>
       <c r="B41" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="E41" s="7" t="str">
         <f>A$39</f>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="8"/>
@@ -1460,20 +1460,20 @@
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>mvreason:CDENotPresentedDuetoException</v>
+        <v>mvreason:CDENotPresentedDuetoException-9943</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E42" s="7" t="str">
         <f>A$39</f>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="8"/>
@@ -1483,20 +1483,20 @@
     <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>mvreason:ElementNeverPresentedforCollection</v>
+        <v>mvreason:ElementNeverPresentedforCollection-9944</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="E43" s="7" t="str">
         <f t="shared" ref="E43:E44" si="6">A$39</f>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="8"/>
@@ -1506,20 +1506,20 @@
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="str">
         <f t="shared" ref="A44" si="7">IF(ISBLANK($B44),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B44," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:ProcessError</v>
+        <v>mvreason:ProcessError-9945</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="C44" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="E44" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="8"/>
@@ -1529,20 +1529,20 @@
     <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="str">
         <f t="shared" ref="A45" si="8">IF(ISBLANK($B45),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B45," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>mvreason:OtherUnpresentedReasonNotSpecified</v>
+        <v>mvreason:OtherUnpresentedReasonNotSpecified-9946</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="E45" s="7" t="str">
         <f t="shared" ref="E45" si="9">A$39</f>
-        <v>mvreason:NotPresentedtoParticipant</v>
+        <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="8"/>

</xml_diff>

<commit_message>
test:  bump up version number
</commit_message>
<xml_diff>
--- a/mvreason.xlsx
+++ b/mvreason.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/horridge/IdeaProjects/radx-missing-value-reasons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexskr/workspace/radx/radx-missing-value-reasons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77DEAED-D6CB-C04F-AF50-9700B8F5282D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79608572-252B-924C-BA6A-361BAC47BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -95,13 +98,7 @@
     <t>pav:lastUpdatedOn</t>
   </si>
   <si>
-    <t>2022-03-23T15:01:00-08:00</t>
-  </si>
-  <si>
     <t>pav:version</t>
-  </si>
-  <si>
-    <t>0.0.5</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -360,6 +357,12 @@
   </si>
   <si>
     <t>The value is missing</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>2024-01-12T15:01:00-08:00</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1144,7 +1147,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1173,13 +1176,13 @@
     </row>
     <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1235,7 +1238,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="3"/>
@@ -1265,7 +1268,7 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
@@ -1295,7 +1298,7 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
@@ -1325,7 +1328,7 @@
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -1411,31 +1414,31 @@
     </row>
     <row r="20" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1461,17 +1464,17 @@
         <v>mvreason:MissingValue-9999</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="12">
         <v>0</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -1500,20 +1503,20 @@
         <v>mvreason:NotSenttoDataHub-9980</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="12">
         <v>1</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="13" t="str">
         <f>A$21</f>
         <v>mvreason:MissingValue-9999</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
@@ -1542,13 +1545,13 @@
         <v>mvreason:DataTransferAgreement-9981</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E23" s="17" t="str">
         <f t="shared" ref="E23:E29" si="1">A$22</f>
@@ -1582,13 +1585,13 @@
         <v>mvreason:NoParticipantConsenttoShare-9982</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1622,13 +1625,13 @@
         <v>mvreason:NotAvailableOrMappable-9983</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E25" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1662,13 +1665,13 @@
         <v>mvreason:DataLostOrInaccessible-9984</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E26" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1702,13 +1705,13 @@
         <v>mvreason:DataInvalid-9985</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1742,13 +1745,13 @@
         <v>mvreason:AnonymizationOrPrivacyConcerns-9986</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1782,13 +1785,13 @@
         <v>mvreason:OtherUnsentReasonNotSpecified-9987</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E29" s="17" t="str">
         <f t="shared" si="1"/>
@@ -1822,24 +1825,24 @@
         <v>mvreason:NotEnteredByOriginator-9960</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="12">
         <v>2</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E30" s="13" t="str">
         <f>A$21</f>
         <v>mvreason:MissingValue-9999</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="3"/>
@@ -1866,13 +1869,13 @@
         <v>mvreason:OmittedThisValue-9961</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="17" t="str">
         <f>A$30</f>
@@ -1906,13 +1909,13 @@
         <v>mvreason:OriginatorChosetoOmit-9962</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" s="17" t="str">
         <f t="shared" ref="E32:E34" si="2">A$31</f>
@@ -1946,13 +1949,13 @@
         <v>mvreason:QuestionNotApplicable-9963</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E33" s="17" t="str">
         <f t="shared" si="2"/>
@@ -1986,13 +1989,13 @@
         <v>mvreason:AnswerNotKnown-9964</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="17" t="str">
         <f t="shared" si="2"/>
@@ -2026,13 +2029,13 @@
         <v>mvreason:RecordNotProvided-9965</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E35" s="17" t="str">
         <f t="shared" ref="E35:E38" si="3">A$30</f>
@@ -2066,13 +2069,13 @@
         <v>mvreason:AllOriginatorsOmittedElement-9966</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E36" s="17" t="str">
         <f t="shared" si="3"/>
@@ -2106,13 +2109,13 @@
         <v>mvreason:CDEOmittedwithException-9967</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E37" s="17" t="str">
         <f t="shared" si="3"/>
@@ -2146,13 +2149,13 @@
         <v>mvreason:OtherUnenteredReasonNotSpecified-9968</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E38" s="17" t="str">
         <f t="shared" si="3"/>
@@ -2186,24 +2189,24 @@
         <v>mvreason:NotPresentedtoParticipant-9940</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="26">
         <v>3</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E39" s="13" t="str">
         <f>A$21</f>
         <v>mvreason:MissingValue-9999</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G39" s="27"/>
       <c r="H39" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="3"/>
@@ -2230,13 +2233,13 @@
         <v>mvreason:SkipLogic-9941</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E40" s="17" t="str">
         <f t="shared" ref="E40:E45" si="4">A$39</f>
@@ -2270,13 +2273,13 @@
         <v>mvreason:NoParticipantConsenttoAsk-9942</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E41" s="17" t="str">
         <f t="shared" si="4"/>
@@ -2310,13 +2313,13 @@
         <v>mvreason:CDENotPresentedDuetoException-9943</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E42" s="17" t="str">
         <f t="shared" si="4"/>
@@ -2350,13 +2353,13 @@
         <v>mvreason:ElementNeverPresentedforCollection-9944</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E43" s="17" t="str">
         <f t="shared" si="4"/>
@@ -2390,13 +2393,13 @@
         <v>mvreason:ProcessError-9945</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E44" s="17" t="str">
         <f t="shared" si="4"/>
@@ -2430,13 +2433,13 @@
         <v>mvreason:OtherUnpresentedReasonNotSpecified-9946</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E45" s="17" t="str">
         <f t="shared" si="4"/>

</xml_diff>